<commit_message>
login and get the list of employees
</commit_message>
<xml_diff>
--- a/src/test/resources/chataakWebApplicationXpath.xlsx
+++ b/src/test/resources/chataakWebApplicationXpath.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">Key</t>
   </si>
@@ -31,19 +31,19 @@
     <t xml:space="preserve">EmailAddress</t>
   </si>
   <si>
-    <t xml:space="preserve">//input[@placeholder='johndoe@example.com']</t>
+    <t xml:space="preserve">//input[@id='login_username']</t>
   </si>
   <si>
     <t xml:space="preserve">password</t>
   </si>
   <si>
-    <t xml:space="preserve">//input[@placeholder='Password']</t>
+    <t xml:space="preserve">//input[@id='login_password']</t>
   </si>
   <si>
     <t xml:space="preserve">login_Button</t>
   </si>
   <si>
-    <t xml:space="preserve">//button[normalize-space()='Login']</t>
+    <t xml:space="preserve">//button[normalize-space()='Sign in']</t>
   </si>
   <si>
     <t xml:space="preserve">Store_Card_Total_Stores_Name</t>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t xml:space="preserve">//div[contains(@class, 'MuiDataGrid-row')]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logout_Button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//span[normalize-space()='logout']</t>
   </si>
 </sst>
 </file>
@@ -403,10 +409,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -504,25 +510,13 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0"/>
-      <c r="B12" s="0"/>
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="C12" s="7"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0"/>
-      <c r="B13" s="0"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0"/>
-      <c r="B14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0"/>
-      <c r="B15" s="0"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0"/>
-      <c r="B16" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>